<commit_message>
Update DRain volume names after Met Office typo fixes
</commit_message>
<xml_diff>
--- a/Scratch/Daily-Rainfall/PDF_Properties.xlsx
+++ b/Scratch/Daily-Rainfall/PDF_Properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\PDF_Experiments\pdf_list_working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\Scratch\Daily-Rainfall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{354F5003-BA5D-413A-8ED8-803D712E40D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A28643C-49A8-44A6-B7AC-BECDAA893F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21AA7748-3BFB-4CF8-8E18-92843B36CD54}"/>
   </bookViews>
@@ -2497,12 +2497,6 @@
     <t>DRain_1931_Wigtown_To_Argyll_Part2</t>
   </si>
   <si>
-    <t>DRain_1932_Clackmannan_Shetland_Part1</t>
-  </si>
-  <si>
-    <t>DRain_1932_Clackmannan_Shetland_Part2</t>
-  </si>
-  <si>
     <t>DRain_1932_Wigtown_To_Argyll_Part1</t>
   </si>
   <si>
@@ -3037,12 +3031,6 @@
     <t>DRain_1944_Wigtown_To_Argyll_Part2</t>
   </si>
   <si>
-    <t>DRain_1945_Clackmannan_To_Argyll_Part1</t>
-  </si>
-  <si>
-    <t>DRain_1945_Clackmannan_To_Argyll_Part2</t>
-  </si>
-  <si>
     <t>DRain_1945_Wigtown_To_Argyll_Part1</t>
   </si>
   <si>
@@ -3656,6 +3644,18 @@
   </si>
   <si>
     <t>Table of Contents Summary</t>
+  </si>
+  <si>
+    <t>DRain_1945_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>DRain_1945_Clackmannan_To_Shetland_Part1</t>
+  </si>
+  <si>
+    <t>DRain_1932_Clackmannan_To_Shetland_Part2</t>
+  </si>
+  <si>
+    <t>DRain_1932_Clackmannan_To_Shetland_Part1</t>
   </si>
 </sst>
 </file>
@@ -4520,8 +4520,8 @@
   <dimension ref="A1:I1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A642" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4563,7 +4563,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -23123,7 +23123,7 @@
     </row>
     <row r="659" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>824</v>
+        <v>1210</v>
       </c>
       <c r="B659">
         <v>71244342</v>
@@ -23146,7 +23146,7 @@
     </row>
     <row r="660" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>825</v>
+        <v>1209</v>
       </c>
       <c r="B660">
         <v>73174130</v>
@@ -23169,7 +23169,7 @@
     </row>
     <row r="661" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B661">
         <v>96645945</v>
@@ -23192,7 +23192,7 @@
     </row>
     <row r="662" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B662">
         <v>102221899</v>
@@ -23215,7 +23215,7 @@
     </row>
     <row r="663" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B663">
         <v>76968035</v>
@@ -23238,7 +23238,7 @@
     </row>
     <row r="664" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B664">
         <v>78042553</v>
@@ -23261,7 +23261,7 @@
     </row>
     <row r="665" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B665">
         <v>99410924</v>
@@ -23284,7 +23284,7 @@
     </row>
     <row r="666" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B666">
         <v>100849776</v>
@@ -23307,7 +23307,7 @@
     </row>
     <row r="667" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B667">
         <v>69571319</v>
@@ -23330,7 +23330,7 @@
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B668">
         <v>70848889</v>
@@ -23353,7 +23353,7 @@
     </row>
     <row r="669" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B669">
         <v>96275503</v>
@@ -23376,7 +23376,7 @@
     </row>
     <row r="670" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B670">
         <v>99037892</v>
@@ -23399,7 +23399,7 @@
     </row>
     <row r="671" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B671">
         <v>87601318</v>
@@ -23422,7 +23422,7 @@
     </row>
     <row r="672" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B672">
         <v>88282285</v>
@@ -23445,7 +23445,7 @@
     </row>
     <row r="673" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B673">
         <v>115913352</v>
@@ -23468,7 +23468,7 @@
     </row>
     <row r="674" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B674">
         <v>115947727</v>
@@ -23491,7 +23491,7 @@
     </row>
     <row r="675" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B675">
         <v>96039390</v>
@@ -23506,21 +23506,21 @@
         <v>74</v>
       </c>
       <c r="F675" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G675" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H675" t="b">
         <v>0</v>
       </c>
       <c r="I675" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="676" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B676">
         <v>95384838</v>
@@ -23535,21 +23535,21 @@
         <v>74</v>
       </c>
       <c r="F676" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G676" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H676" t="b">
         <v>0</v>
       </c>
       <c r="I676" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="677" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B677">
         <v>129710342</v>
@@ -23564,21 +23564,21 @@
         <v>74</v>
       </c>
       <c r="F677" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G677" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H677" t="b">
         <v>0</v>
       </c>
       <c r="I677" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B678">
         <v>129442928</v>
@@ -23593,21 +23593,21 @@
         <v>74</v>
       </c>
       <c r="F678" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G678" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H678" t="b">
         <v>0</v>
       </c>
       <c r="I678" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="679" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B679">
         <v>90442761</v>
@@ -23622,21 +23622,21 @@
         <v>74</v>
       </c>
       <c r="F679" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G679" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H679" t="b">
         <v>0</v>
       </c>
       <c r="I679" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="680" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B680">
         <v>89927362</v>
@@ -23651,21 +23651,21 @@
         <v>74</v>
       </c>
       <c r="F680" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="G680" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="H680" t="b">
         <v>0</v>
       </c>
       <c r="I680" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="681" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B681">
         <v>130883142</v>
@@ -23688,7 +23688,7 @@
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B682">
         <v>131631576</v>
@@ -23711,7 +23711,7 @@
     </row>
     <row r="683" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B683">
         <v>91408699</v>
@@ -23734,7 +23734,7 @@
     </row>
     <row r="684" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B684">
         <v>91827956</v>
@@ -23757,7 +23757,7 @@
     </row>
     <row r="685" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B685">
         <v>118690101</v>
@@ -23780,7 +23780,7 @@
     </row>
     <row r="686" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B686">
         <v>119084867</v>
@@ -23803,7 +23803,7 @@
     </row>
     <row r="687" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B687">
         <v>78098885</v>
@@ -23826,7 +23826,7 @@
     </row>
     <row r="688" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B688">
         <v>78362375</v>
@@ -23849,7 +23849,7 @@
     </row>
     <row r="689" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B689">
         <v>111630778</v>
@@ -23872,7 +23872,7 @@
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B690">
         <v>112148831</v>
@@ -23895,7 +23895,7 @@
     </row>
     <row r="691" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B691">
         <v>77684923</v>
@@ -23918,7 +23918,7 @@
     </row>
     <row r="692" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B692">
         <v>78227833</v>
@@ -23941,7 +23941,7 @@
     </row>
     <row r="693" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B693">
         <v>97587627</v>
@@ -23964,7 +23964,7 @@
     </row>
     <row r="694" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B694">
         <v>97090365</v>
@@ -23987,7 +23987,7 @@
     </row>
     <row r="695" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="B695">
         <v>40164423</v>
@@ -24016,7 +24016,7 @@
     </row>
     <row r="696" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B696">
         <v>51809558</v>
@@ -24045,7 +24045,7 @@
     </row>
     <row r="697" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B697">
         <v>42420047</v>
@@ -24074,7 +24074,7 @@
     </row>
     <row r="698" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B698">
         <v>46391841</v>
@@ -24103,7 +24103,7 @@
     </row>
     <row r="699" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B699">
         <v>37051422</v>
@@ -24132,7 +24132,7 @@
     </row>
     <row r="700" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B700">
         <v>39582271</v>
@@ -24161,7 +24161,7 @@
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B701">
         <v>38607560</v>
@@ -24190,7 +24190,7 @@
     </row>
     <row r="702" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B702">
         <v>43790665</v>
@@ -24219,7 +24219,7 @@
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B703">
         <v>35767809</v>
@@ -24248,7 +24248,7 @@
     </row>
     <row r="704" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="B704">
         <v>39123485</v>
@@ -24277,7 +24277,7 @@
     </row>
     <row r="705" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B705">
         <v>39246716</v>
@@ -24306,7 +24306,7 @@
     </row>
     <row r="706" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B706">
         <v>35178367</v>
@@ -24335,7 +24335,7 @@
     </row>
     <row r="707" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B707">
         <v>42871544</v>
@@ -24364,7 +24364,7 @@
     </row>
     <row r="708" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B708">
         <v>47868753</v>
@@ -24393,7 +24393,7 @@
     </row>
     <row r="709" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B709">
         <v>43280235</v>
@@ -24422,7 +24422,7 @@
     </row>
     <row r="710" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B710">
         <v>42250345</v>
@@ -24451,7 +24451,7 @@
     </row>
     <row r="711" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B711">
         <v>36077058</v>
@@ -24480,7 +24480,7 @@
     </row>
     <row r="712" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B712">
         <v>38871162</v>
@@ -24509,7 +24509,7 @@
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B713">
         <v>43020681</v>
@@ -24538,7 +24538,7 @@
     </row>
     <row r="714" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B714">
         <v>36222625</v>
@@ -24567,7 +24567,7 @@
     </row>
     <row r="715" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B715">
         <v>47825351</v>
@@ -24596,7 +24596,7 @@
     </row>
     <row r="716" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B716">
         <v>48181022</v>
@@ -24625,7 +24625,7 @@
     </row>
     <row r="717" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B717">
         <v>40446133</v>
@@ -24654,7 +24654,7 @@
     </row>
     <row r="718" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B718">
         <v>47945760</v>
@@ -24683,7 +24683,7 @@
     </row>
     <row r="719" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B719">
         <v>47404607</v>
@@ -24712,7 +24712,7 @@
     </row>
     <row r="720" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B720">
         <v>41795671</v>
@@ -24741,7 +24741,7 @@
     </row>
     <row r="721" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B721">
         <v>41095883</v>
@@ -24770,7 +24770,7 @@
     </row>
     <row r="722" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B722">
         <v>41525608</v>
@@ -24799,7 +24799,7 @@
     </row>
     <row r="723" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B723">
         <v>43816208</v>
@@ -24828,7 +24828,7 @@
     </row>
     <row r="724" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B724">
         <v>58516218</v>
@@ -24857,7 +24857,7 @@
     </row>
     <row r="725" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B725">
         <v>49206415</v>
@@ -24886,7 +24886,7 @@
     </row>
     <row r="726" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B726">
         <v>46427473</v>
@@ -24915,7 +24915,7 @@
     </row>
     <row r="727" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B727">
         <v>50996245</v>
@@ -24944,7 +24944,7 @@
     </row>
     <row r="728" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B728">
         <v>28106355</v>
@@ -24968,12 +24968,12 @@
         <v>1</v>
       </c>
       <c r="I728" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="729" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B729">
         <v>43666083</v>
@@ -25002,7 +25002,7 @@
     </row>
     <row r="730" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B730">
         <v>38839288</v>
@@ -25031,7 +25031,7 @@
     </row>
     <row r="731" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B731">
         <v>48198077</v>
@@ -25060,7 +25060,7 @@
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B732">
         <v>14511138</v>
@@ -25084,12 +25084,12 @@
         <v>1</v>
       </c>
       <c r="I732" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B733">
         <v>50676949</v>
@@ -25118,7 +25118,7 @@
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B734">
         <v>53309577</v>
@@ -25147,7 +25147,7 @@
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B735">
         <v>54133487</v>
@@ -25176,7 +25176,7 @@
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B736">
         <v>45558009</v>
@@ -25205,7 +25205,7 @@
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B737">
         <v>48150749</v>
@@ -25234,7 +25234,7 @@
     </row>
     <row r="738" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B738">
         <v>38834252</v>
@@ -25263,7 +25263,7 @@
     </row>
     <row r="739" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B739">
         <v>43523145</v>
@@ -25292,7 +25292,7 @@
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B740">
         <v>31964839</v>
@@ -25321,7 +25321,7 @@
     </row>
     <row r="741" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B741">
         <v>42540243</v>
@@ -25350,7 +25350,7 @@
     </row>
     <row r="742" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B742">
         <v>34900053</v>
@@ -25379,7 +25379,7 @@
     </row>
     <row r="743" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B743">
         <v>38957356</v>
@@ -25408,7 +25408,7 @@
     </row>
     <row r="744" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B744">
         <v>41203057</v>
@@ -25437,7 +25437,7 @@
     </row>
     <row r="745" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B745">
         <v>41401597</v>
@@ -25466,7 +25466,7 @@
     </row>
     <row r="746" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="B746">
         <v>29722604</v>
@@ -25495,7 +25495,7 @@
     </row>
     <row r="747" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B747">
         <v>50804189</v>
@@ -25524,7 +25524,7 @@
     </row>
     <row r="748" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B748">
         <v>38852548</v>
@@ -25553,7 +25553,7 @@
     </row>
     <row r="749" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B749">
         <v>47322036</v>
@@ -25582,7 +25582,7 @@
     </row>
     <row r="750" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B750">
         <v>46445894</v>
@@ -25611,7 +25611,7 @@
     </row>
     <row r="751" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B751">
         <v>38148978</v>
@@ -25640,7 +25640,7 @@
     </row>
     <row r="752" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="B752">
         <v>47431439</v>
@@ -25669,7 +25669,7 @@
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B753">
         <v>45132160</v>
@@ -25698,7 +25698,7 @@
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="B754">
         <v>41691343</v>
@@ -25727,7 +25727,7 @@
     </row>
     <row r="755" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="B755">
         <v>41084394</v>
@@ -25756,7 +25756,7 @@
     </row>
     <row r="756" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B756">
         <v>50106954</v>
@@ -25785,7 +25785,7 @@
     </row>
     <row r="757" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B757">
         <v>52016518</v>
@@ -25814,7 +25814,7 @@
     </row>
     <row r="758" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B758">
         <v>48347490</v>
@@ -25843,7 +25843,7 @@
     </row>
     <row r="759" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B759">
         <v>49518456</v>
@@ -25872,7 +25872,7 @@
     </row>
     <row r="760" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B760">
         <v>43799003</v>
@@ -25901,7 +25901,7 @@
     </row>
     <row r="761" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B761">
         <v>55502550</v>
@@ -25930,7 +25930,7 @@
     </row>
     <row r="762" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B762">
         <v>58953930</v>
@@ -25959,7 +25959,7 @@
     </row>
     <row r="763" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B763">
         <v>46366008</v>
@@ -25988,7 +25988,7 @@
     </row>
     <row r="764" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B764">
         <v>54324453</v>
@@ -26017,7 +26017,7 @@
     </row>
     <row r="765" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B765">
         <v>52129549</v>
@@ -26046,7 +26046,7 @@
     </row>
     <row r="766" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B766">
         <v>50313454</v>
@@ -26075,7 +26075,7 @@
     </row>
     <row r="767" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B767">
         <v>62005153</v>
@@ -26104,7 +26104,7 @@
     </row>
     <row r="768" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B768">
         <v>60824587</v>
@@ -26133,7 +26133,7 @@
     </row>
     <row r="769" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B769">
         <v>46397847</v>
@@ -26162,7 +26162,7 @@
     </row>
     <row r="770" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B770">
         <v>49962115</v>
@@ -26191,7 +26191,7 @@
     </row>
     <row r="771" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B771">
         <v>60450540</v>
@@ -26220,7 +26220,7 @@
     </row>
     <row r="772" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B772">
         <v>47831933</v>
@@ -26249,7 +26249,7 @@
     </row>
     <row r="773" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B773">
         <v>39292828</v>
@@ -26278,7 +26278,7 @@
     </row>
     <row r="774" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B774">
         <v>37407736</v>
@@ -26307,7 +26307,7 @@
     </row>
     <row r="775" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B775">
         <v>47360001</v>
@@ -26336,7 +26336,7 @@
     </row>
     <row r="776" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B776">
         <v>52980506</v>
@@ -26365,7 +26365,7 @@
     </row>
     <row r="777" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B777">
         <v>43812147</v>
@@ -26394,7 +26394,7 @@
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B778">
         <v>44387369</v>
@@ -26423,7 +26423,7 @@
     </row>
     <row r="779" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B779">
         <v>38451649</v>
@@ -26447,12 +26447,12 @@
         <v>1</v>
       </c>
       <c r="I779" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="780" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B780">
         <v>45689682</v>
@@ -26481,7 +26481,7 @@
     </row>
     <row r="781" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B781">
         <v>46560520</v>
@@ -26510,7 +26510,7 @@
     </row>
     <row r="782" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B782">
         <v>48311101</v>
@@ -26539,7 +26539,7 @@
     </row>
     <row r="783" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B783">
         <v>38915700</v>
@@ -26568,7 +26568,7 @@
     </row>
     <row r="784" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B784">
         <v>33895031</v>
@@ -26592,12 +26592,12 @@
         <v>1</v>
       </c>
       <c r="I784" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="785" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B785">
         <v>43475165</v>
@@ -26621,12 +26621,12 @@
         <v>1</v>
       </c>
       <c r="I785" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="786" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B786">
         <v>51174900</v>
@@ -26655,7 +26655,7 @@
     </row>
     <row r="787" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B787">
         <v>44681120</v>
@@ -26684,7 +26684,7 @@
     </row>
     <row r="788" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="B788">
         <v>51821106</v>
@@ -26713,7 +26713,7 @@
     </row>
     <row r="789" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="B789">
         <v>39033280</v>
@@ -26742,7 +26742,7 @@
     </row>
     <row r="790" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B790">
         <v>41890061</v>
@@ -26771,7 +26771,7 @@
     </row>
     <row r="791" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="B791">
         <v>55577262</v>
@@ -26800,7 +26800,7 @@
     </row>
     <row r="792" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B792">
         <v>44254139</v>
@@ -26829,7 +26829,7 @@
     </row>
     <row r="793" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B793">
         <v>43765032</v>
@@ -26858,7 +26858,7 @@
     </row>
     <row r="794" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B794">
         <v>51753189</v>
@@ -26887,7 +26887,7 @@
     </row>
     <row r="795" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B795">
         <v>54209660</v>
@@ -26916,7 +26916,7 @@
     </row>
     <row r="796" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B796">
         <v>39717438</v>
@@ -26945,7 +26945,7 @@
     </row>
     <row r="797" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B797">
         <v>41490257</v>
@@ -26974,7 +26974,7 @@
     </row>
     <row r="798" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B798">
         <v>41595625</v>
@@ -27003,7 +27003,7 @@
     </row>
     <row r="799" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B799">
         <v>57714456</v>
@@ -27032,7 +27032,7 @@
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B800">
         <v>64344948</v>
@@ -27061,7 +27061,7 @@
     </row>
     <row r="801" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B801">
         <v>59535329</v>
@@ -27090,7 +27090,7 @@
     </row>
     <row r="802" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B802">
         <v>68181438</v>
@@ -27119,7 +27119,7 @@
     </row>
     <row r="803" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B803">
         <v>58811995</v>
@@ -27148,7 +27148,7 @@
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B804">
         <v>62672879</v>
@@ -27177,7 +27177,7 @@
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B805">
         <v>59417149</v>
@@ -27206,7 +27206,7 @@
     </row>
     <row r="806" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B806">
         <v>50973898</v>
@@ -27235,7 +27235,7 @@
     </row>
     <row r="807" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B807">
         <v>48167267</v>
@@ -27264,7 +27264,7 @@
     </row>
     <row r="808" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B808">
         <v>53317646</v>
@@ -27293,7 +27293,7 @@
     </row>
     <row r="809" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B809">
         <v>55447733</v>
@@ -27322,7 +27322,7 @@
     </row>
     <row r="810" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B810">
         <v>45304197</v>
@@ -27351,7 +27351,7 @@
     </row>
     <row r="811" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B811">
         <v>36104440</v>
@@ -27375,12 +27375,12 @@
         <v>1</v>
       </c>
       <c r="I811" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="812" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B812">
         <v>79407013</v>
@@ -27403,7 +27403,7 @@
     </row>
     <row r="813" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B813">
         <v>80546275</v>
@@ -27426,7 +27426,7 @@
     </row>
     <row r="814" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B814">
         <v>102987862</v>
@@ -27449,7 +27449,7 @@
     </row>
     <row r="815" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B815">
         <v>102811473</v>
@@ -27472,7 +27472,7 @@
     </row>
     <row r="816" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B816">
         <v>74985307</v>
@@ -27495,7 +27495,7 @@
     </row>
     <row r="817" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B817">
         <v>77724584</v>
@@ -27518,7 +27518,7 @@
     </row>
     <row r="818" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B818">
         <v>102285241</v>
@@ -27541,7 +27541,7 @@
     </row>
     <row r="819" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B819">
         <v>101919993</v>
@@ -27564,7 +27564,7 @@
     </row>
     <row r="820" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B820">
         <v>87617322</v>
@@ -27587,7 +27587,7 @@
     </row>
     <row r="821" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B821">
         <v>88922947</v>
@@ -27610,7 +27610,7 @@
     </row>
     <row r="822" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B822">
         <v>108762552</v>
@@ -27633,7 +27633,7 @@
     </row>
     <row r="823" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B823">
         <v>109405504</v>
@@ -27656,7 +27656,7 @@
     </row>
     <row r="824" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B824">
         <v>89198127</v>
@@ -27679,7 +27679,7 @@
     </row>
     <row r="825" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B825">
         <v>90201293</v>
@@ -27702,7 +27702,7 @@
     </row>
     <row r="826" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B826">
         <v>102922700</v>
@@ -27725,7 +27725,7 @@
     </row>
     <row r="827" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B827">
         <v>102708219</v>
@@ -27748,7 +27748,7 @@
     </row>
     <row r="828" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>1004</v>
+        <v>1208</v>
       </c>
       <c r="B828">
         <v>88715526</v>
@@ -27771,7 +27771,7 @@
     </row>
     <row r="829" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>1005</v>
+        <v>1207</v>
       </c>
       <c r="B829">
         <v>89627775</v>
@@ -27794,7 +27794,7 @@
     </row>
     <row r="830" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="B830">
         <v>103919003</v>
@@ -27817,7 +27817,7 @@
     </row>
     <row r="831" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="B831">
         <v>104223855</v>
@@ -27840,7 +27840,7 @@
     </row>
     <row r="832" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="B832">
         <v>87659611</v>
@@ -27863,7 +27863,7 @@
     </row>
     <row r="833" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="B833">
         <v>89045990</v>
@@ -27886,7 +27886,7 @@
     </row>
     <row r="834" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="B834">
         <v>106433522</v>
@@ -27909,7 +27909,7 @@
     </row>
     <row r="835" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="B835">
         <v>106151440</v>
@@ -27932,7 +27932,7 @@
     </row>
     <row r="836" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="B836">
         <v>85098894</v>
@@ -27955,7 +27955,7 @@
     </row>
     <row r="837" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="B837">
         <v>85189541</v>
@@ -27978,7 +27978,7 @@
     </row>
     <row r="838" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="B838">
         <v>110619603</v>
@@ -28001,7 +28001,7 @@
     </row>
     <row r="839" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="B839">
         <v>109957976</v>
@@ -28024,7 +28024,7 @@
     </row>
     <row r="840" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="B840">
         <v>86120447</v>
@@ -28047,7 +28047,7 @@
     </row>
     <row r="841" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="B841">
         <v>88717732</v>
@@ -28070,7 +28070,7 @@
     </row>
     <row r="842" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="B842">
         <v>86038745</v>
@@ -28093,7 +28093,7 @@
     </row>
     <row r="843" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="B843">
         <v>87213209</v>
@@ -28116,7 +28116,7 @@
     </row>
     <row r="844" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="B844">
         <v>69437006</v>
@@ -28139,7 +28139,7 @@
     </row>
     <row r="845" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="B845">
         <v>70861253</v>
@@ -28162,7 +28162,7 @@
     </row>
     <row r="846" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="B846">
         <v>90627686</v>
@@ -28185,7 +28185,7 @@
     </row>
     <row r="847" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="B847">
         <v>91847888</v>
@@ -28208,7 +28208,7 @@
     </row>
     <row r="848" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="B848">
         <v>89993228</v>
@@ -28231,7 +28231,7 @@
     </row>
     <row r="849" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="B849">
         <v>89137083</v>
@@ -28254,7 +28254,7 @@
     </row>
     <row r="850" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="B850">
         <v>91762856</v>
@@ -28277,7 +28277,7 @@
     </row>
     <row r="851" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="B851">
         <v>90158345</v>
@@ -28300,7 +28300,7 @@
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="B852">
         <v>87087819</v>
@@ -28323,7 +28323,7 @@
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="B853">
         <v>86496353</v>
@@ -28346,7 +28346,7 @@
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="B854">
         <v>96469531</v>
@@ -28369,7 +28369,7 @@
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="B855">
         <v>96205638</v>
@@ -28392,7 +28392,7 @@
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="B856">
         <v>68858099</v>
@@ -28416,12 +28416,12 @@
         <v>0</v>
       </c>
       <c r="I856" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="B857">
         <v>66693970</v>
@@ -28445,12 +28445,12 @@
         <v>0</v>
       </c>
       <c r="I857" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="858" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="B858">
         <v>88452359</v>
@@ -28473,7 +28473,7 @@
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="B859">
         <v>89715655</v>
@@ -28496,7 +28496,7 @@
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="B860">
         <v>88716153</v>
@@ -28519,7 +28519,7 @@
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="B861">
         <v>88604853</v>
@@ -28542,7 +28542,7 @@
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="B862">
         <v>106692654</v>
@@ -28565,7 +28565,7 @@
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="B863">
         <v>106272202</v>
@@ -28588,7 +28588,7 @@
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="B864">
         <v>84332960</v>
@@ -28611,7 +28611,7 @@
     </row>
     <row r="865" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="B865">
         <v>85231641</v>
@@ -28634,7 +28634,7 @@
     </row>
     <row r="866" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="B866">
         <v>101786695</v>
@@ -28657,7 +28657,7 @@
     </row>
     <row r="867" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="B867">
         <v>100048217</v>
@@ -28680,7 +28680,7 @@
     </row>
     <row r="868" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="B868">
         <v>81684403</v>
@@ -28704,12 +28704,12 @@
         <v>0</v>
       </c>
       <c r="I868" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="869" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="B869">
         <v>80570617</v>
@@ -28733,12 +28733,12 @@
         <v>0</v>
       </c>
       <c r="I869" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="870" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="B870">
         <v>105873842</v>
@@ -28761,7 +28761,7 @@
     </row>
     <row r="871" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="B871">
         <v>107241144</v>
@@ -28784,7 +28784,7 @@
     </row>
     <row r="872" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="B872">
         <v>81190698</v>
@@ -28807,7 +28807,7 @@
     </row>
     <row r="873" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="B873">
         <v>82552107</v>
@@ -28830,7 +28830,7 @@
     </row>
     <row r="874" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="B874">
         <v>108476625</v>
@@ -28853,7 +28853,7 @@
     </row>
     <row r="875" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="B875">
         <v>110376524</v>
@@ -28876,7 +28876,7 @@
     </row>
     <row r="876" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="B876">
         <v>88637041</v>
@@ -28899,7 +28899,7 @@
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="B877">
         <v>91864284</v>
@@ -28922,7 +28922,7 @@
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="B878">
         <v>103617943</v>
@@ -28945,7 +28945,7 @@
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="B879">
         <v>103391561</v>
@@ -28968,7 +28968,7 @@
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="B880">
         <v>92379778</v>
@@ -28991,7 +28991,7 @@
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="B881">
         <v>93472187</v>
@@ -29014,7 +29014,7 @@
     </row>
     <row r="882" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="B882">
         <v>103172281</v>
@@ -29037,7 +29037,7 @@
     </row>
     <row r="883" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="B883">
         <v>101917838</v>
@@ -29060,7 +29060,7 @@
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="B884">
         <v>97492951</v>
@@ -29083,7 +29083,7 @@
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="B885">
         <v>102115084</v>
@@ -29106,7 +29106,7 @@
     </row>
     <row r="886" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="B886">
         <v>122337000</v>
@@ -29129,7 +29129,7 @@
     </row>
     <row r="887" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="B887">
         <v>120413246</v>
@@ -29152,7 +29152,7 @@
     </row>
     <row r="888" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="B888">
         <v>106575162</v>
@@ -29175,7 +29175,7 @@
     </row>
     <row r="889" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="B889">
         <v>108352530</v>
@@ -29198,7 +29198,7 @@
     </row>
     <row r="890" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="B890">
         <v>107465680</v>
@@ -29221,7 +29221,7 @@
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="B891">
         <v>109274119</v>
@@ -29244,7 +29244,7 @@
     </row>
     <row r="892" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="B892">
         <v>50059316</v>
@@ -29268,12 +29268,12 @@
         <v>1</v>
       </c>
       <c r="I892" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="B893">
         <v>61797779</v>
@@ -29302,7 +29302,7 @@
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="B894">
         <v>64646064</v>
@@ -29331,7 +29331,7 @@
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="B895">
         <v>76940917</v>
@@ -29360,7 +29360,7 @@
     </row>
     <row r="896" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="B896">
         <v>65486170</v>
@@ -29389,7 +29389,7 @@
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="B897">
         <v>66899544</v>
@@ -29418,7 +29418,7 @@
     </row>
     <row r="898" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="B898">
         <v>58542704</v>
@@ -29447,7 +29447,7 @@
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="B899">
         <v>59669234</v>
@@ -29476,7 +29476,7 @@
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="B900">
         <v>61650315</v>
@@ -29505,7 +29505,7 @@
     </row>
     <row r="901" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="B901">
         <v>57996549</v>
@@ -29534,7 +29534,7 @@
     </row>
     <row r="902" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="B902">
         <v>57953056</v>
@@ -29563,7 +29563,7 @@
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="B903">
         <v>58938736</v>
@@ -29592,7 +29592,7 @@
     </row>
     <row r="904" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="B904">
         <v>66569077</v>
@@ -29621,7 +29621,7 @@
     </row>
     <row r="905" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="B905">
         <v>65783003</v>
@@ -29650,7 +29650,7 @@
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="B906">
         <v>66556952</v>
@@ -29679,7 +29679,7 @@
     </row>
     <row r="907" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="B907">
         <v>46262298</v>
@@ -29708,7 +29708,7 @@
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="B908">
         <v>56280561</v>
@@ -29737,7 +29737,7 @@
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="B909">
         <v>53631796</v>
@@ -29766,7 +29766,7 @@
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="B910">
         <v>53789247</v>
@@ -29795,7 +29795,7 @@
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="B911">
         <v>46780173</v>
@@ -29824,7 +29824,7 @@
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B912">
         <v>52050303</v>
@@ -29848,12 +29848,12 @@
         <v>1</v>
       </c>
       <c r="I912" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="913" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="B913">
         <v>63491476</v>
@@ -29882,7 +29882,7 @@
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="B914">
         <v>52740310</v>
@@ -29911,7 +29911,7 @@
     </row>
     <row r="915" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="B915">
         <v>82167864</v>
@@ -29940,7 +29940,7 @@
     </row>
     <row r="916" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B916">
         <v>54986057</v>
@@ -29969,7 +29969,7 @@
     </row>
     <row r="917" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A917" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="B917">
         <v>58530823</v>
@@ -29998,7 +29998,7 @@
     </row>
     <row r="918" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="B918">
         <v>50883702</v>
@@ -30027,7 +30027,7 @@
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="B919">
         <v>47343276</v>
@@ -30056,7 +30056,7 @@
     </row>
     <row r="920" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B920">
         <v>54228544</v>
@@ -30085,7 +30085,7 @@
     </row>
     <row r="921" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="B921">
         <v>49671581</v>
@@ -30114,7 +30114,7 @@
     </row>
     <row r="922" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="B922">
         <v>43183345</v>
@@ -30143,7 +30143,7 @@
     </row>
     <row r="923" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="B923">
         <v>43739423</v>
@@ -30172,7 +30172,7 @@
     </row>
     <row r="924" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B924">
         <v>53745344</v>
@@ -30201,7 +30201,7 @@
     </row>
     <row r="925" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="B925">
         <v>53599059</v>
@@ -30230,7 +30230,7 @@
     </row>
     <row r="926" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A926" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="B926">
         <v>59932514</v>
@@ -30259,7 +30259,7 @@
     </row>
     <row r="927" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A927" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="B927">
         <v>54120616</v>
@@ -30288,7 +30288,7 @@
     </row>
     <row r="928" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A928" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="B928">
         <v>52926099</v>
@@ -30317,7 +30317,7 @@
     </row>
     <row r="929" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A929" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="B929">
         <v>64207152</v>
@@ -30346,7 +30346,7 @@
     </row>
     <row r="930" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A930" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="B930">
         <v>64841369</v>
@@ -30375,7 +30375,7 @@
     </row>
     <row r="931" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A931" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="B931">
         <v>59213448</v>
@@ -30404,7 +30404,7 @@
     </row>
     <row r="932" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A932" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="B932">
         <v>54434375</v>
@@ -30433,7 +30433,7 @@
     </row>
     <row r="933" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A933" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="B933">
         <v>55819737</v>
@@ -30462,7 +30462,7 @@
     </row>
     <row r="934" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A934" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="B934">
         <v>55189835</v>
@@ -30491,7 +30491,7 @@
     </row>
     <row r="935" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A935" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="B935">
         <v>67124033</v>
@@ -30520,7 +30520,7 @@
     </row>
     <row r="936" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A936" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="B936">
         <v>54118200</v>
@@ -30549,7 +30549,7 @@
     </row>
     <row r="937" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A937" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="B937">
         <v>50050777</v>
@@ -30573,12 +30573,12 @@
         <v>1</v>
       </c>
       <c r="I937" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="938" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A938" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="B938">
         <v>49658554</v>
@@ -30607,7 +30607,7 @@
     </row>
     <row r="939" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A939" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="B939">
         <v>45173374</v>
@@ -30636,7 +30636,7 @@
     </row>
     <row r="940" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A940" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="B940">
         <v>64311802</v>
@@ -30665,7 +30665,7 @@
     </row>
     <row r="941" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A941" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="B941">
         <v>54206538</v>
@@ -30694,7 +30694,7 @@
     </row>
     <row r="942" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A942" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="B942">
         <v>75650733</v>
@@ -30723,7 +30723,7 @@
     </row>
     <row r="943" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A943" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="B943">
         <v>72914923</v>
@@ -30752,7 +30752,7 @@
     </row>
     <row r="944" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A944" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="B944">
         <v>51107183</v>
@@ -30781,7 +30781,7 @@
     </row>
     <row r="945" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A945" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="B945">
         <v>70301681</v>
@@ -30810,7 +30810,7 @@
     </row>
     <row r="946" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A946" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="B946">
         <v>58927646</v>
@@ -30839,7 +30839,7 @@
     </row>
     <row r="947" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A947" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="B947">
         <v>42103674</v>
@@ -30868,7 +30868,7 @@
     </row>
     <row r="948" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A948" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="B948">
         <v>57764997</v>
@@ -30897,7 +30897,7 @@
     </row>
     <row r="949" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A949" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="B949">
         <v>49142875</v>
@@ -30926,7 +30926,7 @@
     </row>
     <row r="950" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A950" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="B950">
         <v>49258209</v>
@@ -30955,7 +30955,7 @@
     </row>
     <row r="951" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A951" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="B951">
         <v>59893559</v>
@@ -30984,7 +30984,7 @@
     </row>
     <row r="952" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="B952">
         <v>69625318</v>
@@ -31013,7 +31013,7 @@
     </row>
     <row r="953" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A953" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="B953">
         <v>63375787</v>
@@ -31042,7 +31042,7 @@
     </row>
     <row r="954" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A954" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="B954">
         <v>61648587</v>
@@ -31071,7 +31071,7 @@
     </row>
     <row r="955" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A955" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="B955">
         <v>47294814</v>
@@ -31100,7 +31100,7 @@
     </row>
     <row r="956" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A956" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="B956">
         <v>59815026</v>
@@ -31129,7 +31129,7 @@
     </row>
     <row r="957" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A957" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="B957">
         <v>60166516</v>
@@ -31158,7 +31158,7 @@
     </row>
     <row r="958" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A958" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="B958">
         <v>53288622</v>
@@ -31187,7 +31187,7 @@
     </row>
     <row r="959" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A959" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="B959">
         <v>66883784</v>
@@ -31216,7 +31216,7 @@
     </row>
     <row r="960" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A960" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="B960">
         <v>65016109</v>
@@ -31245,7 +31245,7 @@
     </row>
     <row r="961" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A961" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="B961">
         <v>51822983</v>
@@ -31274,7 +31274,7 @@
     </row>
     <row r="962" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A962" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="B962">
         <v>50407290</v>
@@ -31303,7 +31303,7 @@
     </row>
     <row r="963" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A963" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="B963">
         <v>62307480</v>
@@ -31332,7 +31332,7 @@
     </row>
     <row r="964" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A964" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="B964">
         <v>52178713</v>
@@ -31361,7 +31361,7 @@
     </row>
     <row r="965" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A965" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="B965">
         <v>52497453</v>
@@ -31390,7 +31390,7 @@
     </row>
     <row r="966" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A966" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="B966">
         <v>71963915</v>
@@ -31419,7 +31419,7 @@
     </row>
     <row r="967" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A967" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="B967">
         <v>44179407</v>
@@ -31443,12 +31443,12 @@
         <v>1</v>
       </c>
       <c r="I967" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="968" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A968" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="B968">
         <v>52551476</v>
@@ -31477,7 +31477,7 @@
     </row>
     <row r="969" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A969" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="B969">
         <v>48626656</v>
@@ -31501,12 +31501,12 @@
         <v>1</v>
       </c>
       <c r="I969" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="970" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A970" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="B970">
         <v>64172968</v>
@@ -31535,7 +31535,7 @@
     </row>
     <row r="971" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A971" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="B971">
         <v>62200140</v>
@@ -31564,7 +31564,7 @@
     </row>
     <row r="972" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A972" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="B972">
         <v>53820383</v>
@@ -31593,7 +31593,7 @@
     </row>
     <row r="973" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A973" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="B973">
         <v>58543894</v>
@@ -31622,7 +31622,7 @@
     </row>
     <row r="974" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A974" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="B974">
         <v>71731481</v>
@@ -31651,7 +31651,7 @@
     </row>
     <row r="975" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A975" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="B975">
         <v>58612114</v>
@@ -31680,7 +31680,7 @@
     </row>
     <row r="976" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A976" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="B976">
         <v>57387839</v>
@@ -31709,7 +31709,7 @@
     </row>
     <row r="977" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A977" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="B977">
         <v>51323998</v>
@@ -31733,12 +31733,12 @@
         <v>1</v>
       </c>
       <c r="I977" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="978" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A978" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="B978">
         <v>57715734</v>
@@ -31767,7 +31767,7 @@
     </row>
     <row r="979" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A979" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="B979">
         <v>60192644</v>
@@ -31796,7 +31796,7 @@
     </row>
     <row r="980" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A980" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="B980">
         <v>58786878</v>
@@ -31825,7 +31825,7 @@
     </row>
     <row r="981" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A981" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="B981">
         <v>60036333</v>
@@ -31854,7 +31854,7 @@
     </row>
     <row r="982" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A982" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="B982">
         <v>69069365</v>
@@ -31883,7 +31883,7 @@
     </row>
     <row r="983" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A983" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="B983">
         <v>60961641</v>
@@ -31912,7 +31912,7 @@
     </row>
     <row r="984" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A984" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="B984">
         <v>59434136</v>
@@ -31941,7 +31941,7 @@
     </row>
     <row r="985" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A985" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="B985">
         <v>62390057</v>
@@ -31970,7 +31970,7 @@
     </row>
     <row r="986" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A986" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="B986">
         <v>60127734</v>
@@ -31999,7 +31999,7 @@
     </row>
     <row r="987" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A987" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="B987">
         <v>65093518</v>
@@ -32028,7 +32028,7 @@
     </row>
     <row r="988" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A988" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="B988">
         <v>58912496</v>
@@ -32057,7 +32057,7 @@
     </row>
     <row r="989" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A989" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="B989">
         <v>67567770</v>
@@ -32086,7 +32086,7 @@
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A990" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="B990">
         <v>65015106</v>
@@ -32115,7 +32115,7 @@
     </row>
     <row r="991" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A991" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="B991">
         <v>45740458</v>
@@ -32139,12 +32139,12 @@
         <v>1</v>
       </c>
       <c r="I991" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="992" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A992" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="B992">
         <v>74125092</v>
@@ -32173,7 +32173,7 @@
     </row>
     <row r="993" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A993" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="B993">
         <v>68952869</v>
@@ -32202,7 +32202,7 @@
     </row>
     <row r="994" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A994" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="B994">
         <v>59664626</v>
@@ -32231,7 +32231,7 @@
     </row>
     <row r="995" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A995" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="B995">
         <v>65167240</v>
@@ -32260,7 +32260,7 @@
     </row>
     <row r="996" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A996" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="B996">
         <v>60518063</v>
@@ -32289,7 +32289,7 @@
     </row>
     <row r="997" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A997" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="B997">
         <v>73389551</v>
@@ -32318,7 +32318,7 @@
     </row>
     <row r="998" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A998" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="B998">
         <v>40501466</v>
@@ -32347,7 +32347,7 @@
     </row>
     <row r="999" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A999" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="B999">
         <v>51664918</v>
@@ -32376,7 +32376,7 @@
     </row>
     <row r="1000" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1000" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="B1000">
         <v>61760681</v>
@@ -32405,7 +32405,7 @@
     </row>
     <row r="1001" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1001" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="B1001">
         <v>49302422</v>
@@ -32434,7 +32434,7 @@
     </row>
     <row r="1002" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1002" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="B1002">
         <v>59756094</v>
@@ -32463,7 +32463,7 @@
     </row>
     <row r="1003" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1003" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="B1003">
         <v>65448511</v>
@@ -32492,7 +32492,7 @@
     </row>
     <row r="1004" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1004" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="B1004">
         <v>64732370</v>
@@ -32521,7 +32521,7 @@
     </row>
     <row r="1005" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1005" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="B1005">
         <v>53539155</v>
@@ -32550,7 +32550,7 @@
     </row>
     <row r="1006" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1006" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="B1006">
         <v>51370720</v>
@@ -32579,7 +32579,7 @@
     </row>
     <row r="1007" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="B1007">
         <v>52644381</v>
@@ -32608,7 +32608,7 @@
     </row>
     <row r="1008" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1008" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="B1008">
         <v>45034244</v>
@@ -32637,7 +32637,7 @@
     </row>
     <row r="1009" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="B1009">
         <v>37127699</v>
@@ -32661,12 +32661,12 @@
         <v>1</v>
       </c>
       <c r="I1009" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="1010" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B1010">
         <v>62880781</v>
@@ -32695,7 +32695,7 @@
     </row>
     <row r="1011" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1011" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="B1011">
         <v>50838085</v>
@@ -32724,7 +32724,7 @@
     </row>
     <row r="1012" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1012" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="B1012">
         <v>55979301</v>
@@ -32753,7 +32753,7 @@
     </row>
     <row r="1013" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1013" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="B1013">
         <v>47853671</v>
@@ -32782,7 +32782,7 @@
     </row>
     <row r="1014" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1014" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="B1014">
         <v>61374069</v>
@@ -32811,7 +32811,7 @@
     </row>
     <row r="1015" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1015" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="B1015">
         <v>17851489</v>
@@ -32826,10 +32826,10 @@
         <v>9</v>
       </c>
       <c r="F1015" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1015" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1015" t="b">
         <v>1</v>
@@ -32840,7 +32840,7 @@
     </row>
     <row r="1016" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="B1016">
         <v>12134286</v>
@@ -32855,10 +32855,10 @@
         <v>9</v>
       </c>
       <c r="F1016" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1016" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1016" t="b">
         <v>1</v>
@@ -32869,7 +32869,7 @@
     </row>
     <row r="1017" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1017" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B1017">
         <v>14345390</v>
@@ -32884,10 +32884,10 @@
         <v>9</v>
       </c>
       <c r="F1017" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1017" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1017" t="b">
         <v>1</v>
@@ -32898,7 +32898,7 @@
     </row>
     <row r="1018" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1018" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="B1018">
         <v>36761247</v>
@@ -32913,10 +32913,10 @@
         <v>9</v>
       </c>
       <c r="F1018" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1018" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1018" t="b">
         <v>1</v>
@@ -32927,7 +32927,7 @@
     </row>
     <row r="1019" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1019" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="B1019">
         <v>5874967</v>
@@ -32942,10 +32942,10 @@
         <v>9</v>
       </c>
       <c r="F1019" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1019" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1019" t="b">
         <v>1</v>
@@ -32956,7 +32956,7 @@
     </row>
     <row r="1020" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="B1020">
         <v>4726153</v>
@@ -32971,10 +32971,10 @@
         <v>9</v>
       </c>
       <c r="F1020" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1020" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1020" t="b">
         <v>1</v>
@@ -32985,7 +32985,7 @@
     </row>
     <row r="1021" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B1021">
         <v>18530371</v>
@@ -33000,10 +33000,10 @@
         <v>9</v>
       </c>
       <c r="F1021" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1021" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1021" t="b">
         <v>1</v>
@@ -33014,7 +33014,7 @@
     </row>
     <row r="1022" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1022" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="B1022">
         <v>128602142</v>
@@ -33029,10 +33029,10 @@
         <v>9</v>
       </c>
       <c r="F1022" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1022" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1022" t="b">
         <v>1</v>
@@ -33043,7 +33043,7 @@
     </row>
     <row r="1023" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1023" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="B1023">
         <v>23405600</v>
@@ -33058,10 +33058,10 @@
         <v>9</v>
       </c>
       <c r="F1023" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1023" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1023" t="b">
         <v>1</v>
@@ -33072,7 +33072,7 @@
     </row>
     <row r="1024" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1024" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="B1024">
         <v>33193764</v>
@@ -33087,10 +33087,10 @@
         <v>9</v>
       </c>
       <c r="F1024" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1024" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1024" t="b">
         <v>1</v>
@@ -33101,7 +33101,7 @@
     </row>
     <row r="1025" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1025" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B1025">
         <v>2263503</v>
@@ -33116,10 +33116,10 @@
         <v>9</v>
       </c>
       <c r="F1025" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1025" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1025" t="b">
         <v>1</v>
@@ -33130,7 +33130,7 @@
     </row>
     <row r="1026" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1026" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="B1026">
         <v>7341243</v>
@@ -33145,10 +33145,10 @@
         <v>9</v>
       </c>
       <c r="F1026" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1026" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1026" t="b">
         <v>1</v>
@@ -33159,7 +33159,7 @@
     </row>
     <row r="1027" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="B1027">
         <v>24059681</v>
@@ -33174,10 +33174,10 @@
         <v>9</v>
       </c>
       <c r="F1027" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1027" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1027" t="b">
         <v>1</v>
@@ -33188,7 +33188,7 @@
     </row>
     <row r="1028" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="B1028">
         <v>28726782</v>
@@ -33203,16 +33203,16 @@
         <v>9</v>
       </c>
       <c r="F1028" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G1028" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="H1028" t="b">
         <v>1</v>
       </c>
       <c r="I1028" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>